<commit_message>
Added Neural Nw, Ridge and Lasso
</commit_message>
<xml_diff>
--- a/TestData/T1.xlsx
+++ b/TestData/T1.xlsx
@@ -116,7 +116,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,21 +138,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -266,7 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,8 +271,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -308,10 +304,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,10 +412,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +519,7 @@
       <c r="A9" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="10" t="n">
@@ -541,7 +533,7 @@
       <c r="A10" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="10" t="n">
@@ -555,7 +547,7 @@
       <c r="A11" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="10" t="n">
@@ -569,7 +561,7 @@
       <c r="A12" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="10" t="n">
@@ -580,26 +572,26 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="15" t="n">
+      <c r="C13" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>